<commit_message>
Finalizado o exercício do Claude para a Aula 2
</commit_message>
<xml_diff>
--- a/Aula_2/beneficios_consolidado.xlsx
+++ b/Aula_2/beneficios_consolidado.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,20 +449,15 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>tipo_beneficio_desconto</t>
+          <t>percentual_desconto</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>percentual_desconto</t>
+          <t>valor_desconto</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
-        <is>
-          <t>valor_desconto</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
         <is>
           <t>valor_liquido</t>
         </is>
@@ -492,18 +487,13 @@
       <c r="E2" t="n">
         <v>850</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>VR</t>
-        </is>
+      <c r="F2" t="n">
+        <v>0.05</v>
       </c>
       <c r="G2" t="n">
-        <v>0.05</v>
+        <v>42.5</v>
       </c>
       <c r="H2" t="n">
-        <v>42.5</v>
-      </c>
-      <c r="I2" t="n">
         <v>807.5</v>
       </c>
     </row>
@@ -531,18 +521,13 @@
       <c r="E3" t="n">
         <v>1125</v>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>VA</t>
-        </is>
+      <c r="F3" t="n">
+        <v>0.03</v>
       </c>
       <c r="G3" t="n">
-        <v>0.03</v>
+        <v>33.75</v>
       </c>
       <c r="H3" t="n">
-        <v>33.75</v>
-      </c>
-      <c r="I3" t="n">
         <v>1091.25</v>
       </c>
     </row>
@@ -570,18 +555,13 @@
       <c r="E4" t="n">
         <v>2500</v>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Plano de Saúde</t>
-        </is>
+      <c r="F4" t="n">
+        <v>0.12</v>
       </c>
       <c r="G4" t="n">
-        <v>0.12</v>
+        <v>300</v>
       </c>
       <c r="H4" t="n">
-        <v>300</v>
-      </c>
-      <c r="I4" t="n">
         <v>2200</v>
       </c>
     </row>
@@ -609,19 +589,14 @@
       <c r="E5" t="n">
         <v>185.29</v>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>VA</t>
-        </is>
+      <c r="F5" t="n">
+        <v>0.05</v>
       </c>
       <c r="G5" t="n">
-        <v>1.12</v>
+        <v>9.26</v>
       </c>
       <c r="H5" t="n">
-        <v>207.52</v>
-      </c>
-      <c r="I5" t="n">
-        <v>-22.23</v>
+        <v>176.03</v>
       </c>
     </row>
     <row r="6">
@@ -648,19 +623,14 @@
       <c r="E6" t="n">
         <v>1113.25</v>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Plano de Saúde</t>
-        </is>
+      <c r="F6" t="n">
+        <v>0.05</v>
       </c>
       <c r="G6" t="n">
-        <v>2.12</v>
+        <v>55.66</v>
       </c>
       <c r="H6" t="n">
-        <v>2360.09</v>
-      </c>
-      <c r="I6" t="n">
-        <v>-1246.84</v>
+        <v>1057.59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>